<commit_message>
update resource by parse tool
</commit_message>
<xml_diff>
--- a/Resource/excel/1000-框架-配置列表.xlsx
+++ b/Resource/excel/1000-框架-配置列表.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="113">
   <si>
     <t>#config</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>./config/drop.xml</t>
+  </si>
+  <si>
+    <t>元素配置表</t>
   </si>
   <si>
     <t>element</t>
@@ -360,10 +363,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -386,37 +389,94 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -429,7 +489,43 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -442,99 +538,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="39">
     <fill>
@@ -581,13 +584,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -599,49 +674,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -653,13 +746,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -672,96 +765,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -786,6 +789,71 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -822,218 +890,153 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="34" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="38" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="18" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1503,7 +1506,7 @@
   <dimension ref="A1:E40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="4"/>
@@ -2033,13 +2036,13 @@
     </row>
     <row r="32" s="9" customFormat="1" spans="1:5">
       <c r="A32" s="9" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B32" s="9" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="D32" s="9">
         <v>1</v>
@@ -2050,13 +2053,13 @@
     </row>
     <row r="33" s="10" customFormat="1" spans="1:5">
       <c r="A33" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="D33" s="10">
         <v>1</v>
@@ -2067,13 +2070,13 @@
     </row>
     <row r="34" s="10" customFormat="1" spans="1:5">
       <c r="A34" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B34" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D34" s="10">
         <v>1</v>
@@ -2084,13 +2087,13 @@
     </row>
     <row r="35" s="10" customFormat="1" spans="1:5">
       <c r="A35" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="D35" s="10">
         <v>1</v>
@@ -2101,13 +2104,13 @@
     </row>
     <row r="36" s="10" customFormat="1" spans="1:5">
       <c r="A36" s="10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="D36" s="10">
         <v>1</v>
@@ -2118,13 +2121,13 @@
     </row>
     <row r="37" s="10" customFormat="1" spans="1:5">
       <c r="A37" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D37" s="10">
         <v>1</v>
@@ -2135,13 +2138,13 @@
     </row>
     <row r="38" s="10" customFormat="1" spans="1:5">
       <c r="A38" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D38" s="10">
         <v>1</v>
@@ -2152,13 +2155,13 @@
     </row>
     <row r="39" s="10" customFormat="1" spans="1:5">
       <c r="A39" s="10" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="D39" s="10">
         <v>1</v>
@@ -2169,13 +2172,13 @@
     </row>
     <row r="40" s="10" customFormat="1" spans="1:5">
       <c r="A40" s="10" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="D40" s="10">
         <v>1</v>

</xml_diff>